<commit_message>
CIERRE 17 ENE 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/INVENTARIO ALMACEN  DICIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/INVENTARIO ALMACEN  DICIEMBRE        2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL#14  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -444,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="120">
   <si>
     <t xml:space="preserve">INVENTARIO GENERAL </t>
   </si>
@@ -842,19 +842,13 @@
     <t>NO REGISTRARON  LA ENTRADA</t>
   </si>
   <si>
-    <t>ERROR DE CAPTURA Y SALIDA</t>
+    <t>error toma de inventario</t>
   </si>
   <si>
-    <t>MAL TOMADO EL INVENTARIO</t>
+    <t>error toma de invenatario</t>
   </si>
   <si>
-    <t>ERROR DE CAPTURA Y MAL TOMADO EL INVENTARIO</t>
-  </si>
-  <si>
-    <t>ERRRO DE ALMACEN EN SALDO</t>
-  </si>
-  <si>
-    <t>ERROR DE CAPTURA EN INICIO DE MES</t>
+    <t>ERROR CAPTURA ALMACEN</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1237,12 +1231,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2188,7 +2176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="406">
+  <cellXfs count="405">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2948,192 +2936,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3146,7 +2948,6 @@
     <xf numFmtId="2" fontId="9" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="13" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="9" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3155,6 +2956,192 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3512,10 +3499,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="346" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="346"/>
+      <c r="A1" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="343"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -3525,10 +3512,10 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="347" t="s">
+      <c r="A2" s="344" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="348"/>
+      <c r="B2" s="345"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3542,32 +3529,32 @@
     </row>
     <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="349" t="s">
+      <c r="B3" s="346" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="350"/>
+      <c r="C3" s="347"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="351" t="s">
+      <c r="E3" s="348" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="352"/>
+      <c r="F3" s="349"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="353" t="s">
+      <c r="H3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="338" t="s">
+      <c r="J3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="339"/>
-      <c r="L3" s="334" t="s">
+      <c r="K3" s="358"/>
+      <c r="L3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="335"/>
-      <c r="N3" s="336" t="s">
+      <c r="M3" s="354"/>
+      <c r="N3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="337"/>
+      <c r="O3" s="356"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -3589,7 +3576,7 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="354"/>
+      <c r="H4" s="351"/>
       <c r="I4" s="11"/>
       <c r="J4" s="16" t="s">
         <v>10</v>
@@ -3862,10 +3849,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="340" t="s">
+      <c r="N11" s="359" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="341"/>
+      <c r="O11" s="360"/>
     </row>
     <row r="12" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
@@ -4035,10 +4022,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N16" s="342" t="s">
+      <c r="N16" s="361" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="343"/>
+      <c r="O16" s="362"/>
     </row>
     <row r="17" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
@@ -4115,10 +4102,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="344" t="s">
+      <c r="N18" s="363" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="345"/>
+      <c r="O18" s="364"/>
     </row>
     <row r="19" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
@@ -4614,10 +4601,10 @@
     <row r="34" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="70"/>
       <c r="C34" s="72"/>
-      <c r="E34" s="333" t="s">
+      <c r="E34" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="333"/>
+      <c r="F34" s="352"/>
       <c r="G34" s="73">
         <f>SUM(G5:G27)</f>
         <v>68686.460000000006</v>
@@ -4642,11 +4629,6 @@
     <sortCondition ref="A10:A28"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="H3:H4"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
@@ -4654,6 +4636,11 @@
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N18:O18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="H3:H4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.15748031496062992" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4693,10 +4680,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="390" t="s">
+      <c r="B1" s="393" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="390"/>
+      <c r="C1" s="393"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -4708,15 +4695,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347">
+      <c r="B2" s="344">
         <v>44507</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -4726,32 +4713,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -4773,7 +4760,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -4830,8 +4817,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="391"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="394"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -4869,8 +4856,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="392"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="395"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -4945,8 +4932,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="389"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="392"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
@@ -5023,8 +5010,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="382"/>
-      <c r="P10" s="367"/>
+      <c r="O10" s="396"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="164" t="s">
@@ -5179,8 +5166,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O14" s="383"/>
-      <c r="P14" s="356"/>
+      <c r="O14" s="397"/>
+      <c r="P14" s="366"/>
     </row>
     <row r="15" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
@@ -5342,8 +5329,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O19" s="384"/>
-      <c r="P19" s="358"/>
+      <c r="O19" s="398"/>
+      <c r="P19" s="368"/>
     </row>
     <row r="20" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
@@ -5412,8 +5399,8 @@
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
-      <c r="O21" s="385"/>
-      <c r="P21" s="363"/>
+      <c r="O21" s="399"/>
+      <c r="P21" s="373"/>
     </row>
     <row r="22" spans="2:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -5451,8 +5438,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="386"/>
-      <c r="P22" s="387"/>
+      <c r="O22" s="400"/>
+      <c r="P22" s="401"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
@@ -5552,8 +5539,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O25" s="388"/>
-      <c r="P25" s="371"/>
+      <c r="O25" s="402"/>
+      <c r="P25" s="381"/>
     </row>
     <row r="26" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
@@ -5905,10 +5892,10 @@
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="333" t="s">
+      <c r="F37" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="333"/>
+      <c r="G37" s="352"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>60036.020000000004</v>
@@ -5961,6 +5948,13 @@
     <sortCondition ref="B5:B27"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -5973,13 +5967,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.47244094488188981" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5994,8 +5981,8 @@
   </sheetPr>
   <dimension ref="B1:X41"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6019,10 +6006,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="390" t="s">
+      <c r="B1" s="393" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="390"/>
+      <c r="C1" s="393"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -6034,15 +6021,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="393">
+      <c r="B2" s="403">
         <v>44535</v>
       </c>
-      <c r="C2" s="394"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="404"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -6052,32 +6039,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -6099,7 +6086,7 @@
       <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -6156,8 +6143,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="391"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="394"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -6195,8 +6182,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="392"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="395"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -6275,8 +6262,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="389"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="392"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
@@ -6353,8 +6340,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="382"/>
-      <c r="P10" s="367"/>
+      <c r="O10" s="396"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
@@ -6517,8 +6504,8 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="O14" s="383"/>
-      <c r="P14" s="356"/>
+      <c r="O14" s="397"/>
+      <c r="P14" s="366"/>
       <c r="Q14" s="321" t="s">
         <v>107</v>
       </c>
@@ -6714,8 +6701,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="384"/>
-      <c r="P19" s="358"/>
+      <c r="O19" s="398"/>
+      <c r="P19" s="368"/>
       <c r="S19" s="317"/>
       <c r="T19" s="317"/>
     </row>
@@ -6800,8 +6787,8 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="O21" s="385"/>
-      <c r="P21" s="363"/>
+      <c r="O21" s="399"/>
+      <c r="P21" s="373"/>
       <c r="Q21" s="320" t="s">
         <v>107</v>
       </c>
@@ -6845,8 +6832,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="386"/>
-      <c r="P22" s="387"/>
+      <c r="O22" s="400"/>
+      <c r="P22" s="401"/>
       <c r="S22" s="317"/>
       <c r="T22" s="317"/>
     </row>
@@ -6948,8 +6935,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25" s="388"/>
-      <c r="P25" s="371"/>
+      <c r="O25" s="402"/>
+      <c r="P25" s="381"/>
     </row>
     <row r="26" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
@@ -7321,10 +7308,10 @@
     <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="333" t="s">
+      <c r="F37" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="333"/>
+      <c r="G37" s="352"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>61259.35</v>
@@ -7385,6 +7372,13 @@
     <sortCondition ref="B5:B34"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -7397,13 +7391,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7418,8 +7405,8 @@
   </sheetPr>
   <dimension ref="B1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7443,10 +7430,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="390" t="s">
+      <c r="B1" s="393" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="390"/>
+      <c r="C1" s="393"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -7458,15 +7445,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="393">
+      <c r="B2" s="403">
         <v>44563</v>
       </c>
-      <c r="C2" s="394"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="404"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -7476,32 +7463,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -7523,7 +7510,7 @@
       <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -7580,8 +7567,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="391"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="394"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -7619,8 +7606,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="392"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="395"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -7695,8 +7682,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="389"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="392"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
@@ -7740,8 +7727,8 @@
       </c>
       <c r="O9" s="260"/>
       <c r="P9" s="132"/>
-      <c r="Q9" s="405" t="s">
-        <v>118</v>
+      <c r="Q9" s="342" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7780,8 +7767,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="382"/>
-      <c r="P10" s="367"/>
+      <c r="O10" s="396"/>
+      <c r="P10" s="377"/>
       <c r="Q10" s="317"/>
       <c r="R10" s="317"/>
     </row>
@@ -7912,7 +7899,7 @@
         <v>8960.25</v>
       </c>
       <c r="D14" s="23">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="240"/>
@@ -7923,7 +7910,7 @@
       </c>
       <c r="I14" s="171">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="212">
@@ -7936,15 +7923,13 @@
         <f t="shared" si="1"/>
         <v>-0.23999999999978172</v>
       </c>
-      <c r="N14" s="401">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="383"/>
-      <c r="P14" s="356"/>
-      <c r="Q14" s="395" t="s">
-        <v>117</v>
-      </c>
+      <c r="N14" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="397"/>
+      <c r="P14" s="366"/>
+      <c r="Q14" s="333"/>
       <c r="R14" s="318"/>
       <c r="S14" s="318"/>
       <c r="T14" s="317"/>
@@ -8153,10 +8138,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O19" s="384"/>
-      <c r="P19" s="358"/>
-      <c r="Q19" s="396" t="s">
-        <v>121</v>
+      <c r="O19" s="398"/>
+      <c r="P19" s="368"/>
+      <c r="Q19" s="334" t="s">
+        <v>117</v>
       </c>
       <c r="R19" s="317"/>
       <c r="S19" s="317"/>
@@ -8200,8 +8185,8 @@
       </c>
       <c r="O20" s="268"/>
       <c r="P20" s="148"/>
-      <c r="Q20" s="396" t="s">
-        <v>119</v>
+      <c r="Q20" s="334" t="s">
+        <v>117</v>
       </c>
       <c r="R20" s="319"/>
       <c r="S20" s="319"/>
@@ -8243,10 +8228,10 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="O21" s="385"/>
-      <c r="P21" s="363"/>
-      <c r="Q21" s="396" t="s">
-        <v>119</v>
+      <c r="O21" s="399"/>
+      <c r="P21" s="373"/>
+      <c r="Q21" s="334" t="s">
+        <v>117</v>
       </c>
       <c r="R21" s="311"/>
       <c r="S21" s="311"/>
@@ -8257,7 +8242,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="240">
-        <v>2667.56</v>
+        <v>2666.52</v>
       </c>
       <c r="D22" s="23">
         <v>98</v>
@@ -8267,7 +8252,7 @@
       <c r="G22" s="25"/>
       <c r="H22" s="176">
         <f t="shared" si="0"/>
-        <v>2667.56</v>
+        <v>2666.52</v>
       </c>
       <c r="I22" s="171">
         <f t="shared" si="0"/>
@@ -8280,17 +8265,19 @@
       <c r="L22" s="213">
         <v>96</v>
       </c>
-      <c r="M22" s="402">
-        <f t="shared" si="1"/>
-        <v>-1.0399999999999636</v>
-      </c>
-      <c r="N22" s="403">
+      <c r="M22" s="339">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="340">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="O22" s="386"/>
-      <c r="P22" s="387"/>
-      <c r="Q22" s="317"/>
+      <c r="O22" s="400"/>
+      <c r="P22" s="401"/>
+      <c r="Q22" s="334" t="s">
+        <v>117</v>
+      </c>
       <c r="R22" s="317"/>
       <c r="S22" s="317"/>
       <c r="T22" s="317"/>
@@ -8389,12 +8376,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N25" s="399">
+      <c r="N25" s="337">
         <f>L25-I25</f>
         <v>1</v>
       </c>
-      <c r="O25" s="388"/>
-      <c r="P25" s="371"/>
+      <c r="O25" s="402"/>
+      <c r="P25" s="381"/>
+      <c r="Q25" s="334" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="26" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
@@ -8562,10 +8552,10 @@
       </c>
       <c r="O30" s="274"/>
       <c r="P30" s="93"/>
-      <c r="Q30" s="397" t="s">
+      <c r="Q30" s="335" t="s">
         <v>116</v>
       </c>
-      <c r="R30" s="398"/>
+      <c r="R30" s="336"/>
     </row>
     <row r="31" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="182" t="s">
@@ -8634,7 +8624,7 @@
       <c r="L32" s="213">
         <v>32</v>
       </c>
-      <c r="M32" s="400">
+      <c r="M32" s="338">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -8644,7 +8634,7 @@
       </c>
       <c r="O32" s="276"/>
       <c r="P32" s="198"/>
-      <c r="Q32" s="405" t="s">
+      <c r="Q32" s="342" t="s">
         <v>119</v>
       </c>
     </row>
@@ -8715,7 +8705,7 @@
       <c r="L34" s="213">
         <v>18</v>
       </c>
-      <c r="M34" s="400">
+      <c r="M34" s="338">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -8725,8 +8715,8 @@
       </c>
       <c r="O34" s="278"/>
       <c r="P34" s="200"/>
-      <c r="Q34" s="404" t="s">
-        <v>120</v>
+      <c r="Q34" s="341" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -8792,17 +8782,17 @@
     <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="333" t="s">
+      <c r="F37" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="333"/>
+      <c r="G37" s="352"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
-        <v>57417.440000000002</v>
+        <v>57416.399999999994</v>
       </c>
       <c r="I37" s="74">
         <f>SUM(I5:I30)</f>
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="76">
@@ -8833,6 +8823,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O14:P14"/>
@@ -8840,18 +8842,6 @@
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="O25:P25"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8902,10 +8892,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="346" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="346"/>
+      <c r="A1" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="343"/>
       <c r="G1" s="156"/>
       <c r="H1" s="157"/>
       <c r="I1" s="157"/>
@@ -8917,10 +8907,10 @@
       <c r="O1" s="161"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="347" t="s">
+      <c r="A2" s="344" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="348"/>
+      <c r="B2" s="345"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -8934,32 +8924,32 @@
     </row>
     <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="349" t="s">
+      <c r="B3" s="346" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="350"/>
+      <c r="C3" s="347"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="351" t="s">
+      <c r="E3" s="348" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="352"/>
+      <c r="F3" s="349"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="353" t="s">
+      <c r="H3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="338" t="s">
+      <c r="J3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="339"/>
-      <c r="L3" s="334" t="s">
+      <c r="K3" s="358"/>
+      <c r="L3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="335"/>
-      <c r="N3" s="336" t="s">
+      <c r="M3" s="354"/>
+      <c r="N3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="337"/>
+      <c r="O3" s="356"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -8981,7 +8971,7 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="354"/>
+      <c r="H4" s="351"/>
       <c r="I4" s="11"/>
       <c r="J4" s="16" t="s">
         <v>10</v>
@@ -9244,8 +9234,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="355"/>
-      <c r="O11" s="356"/>
+      <c r="N11" s="365"/>
+      <c r="O11" s="366"/>
     </row>
     <row r="12" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
@@ -9415,8 +9405,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N16" s="357"/>
-      <c r="O16" s="358"/>
+      <c r="N16" s="367"/>
+      <c r="O16" s="368"/>
     </row>
     <row r="17" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
@@ -9493,8 +9483,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="359"/>
-      <c r="O18" s="360"/>
+      <c r="N18" s="369"/>
+      <c r="O18" s="370"/>
     </row>
     <row r="19" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
@@ -9970,10 +9960,10 @@
     <row r="34" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="70"/>
       <c r="C34" s="72"/>
-      <c r="E34" s="333" t="s">
+      <c r="E34" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="333"/>
+      <c r="F34" s="352"/>
       <c r="G34" s="73">
         <f>SUM(G5:G27)</f>
         <v>37848.980000000003</v>
@@ -9998,11 +9988,6 @@
     <sortCondition ref="A6:A28"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N18:O18"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="E34:F34"/>
@@ -10010,6 +9995,11 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N18:O18"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.15748031496062992" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10049,10 +10039,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -10064,15 +10054,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347" t="s">
+      <c r="B2" s="344" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -10082,32 +10072,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -10129,7 +10119,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -10380,8 +10370,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="355"/>
-      <c r="P11" s="356"/>
+      <c r="O11" s="365"/>
+      <c r="P11" s="366"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
@@ -10551,8 +10541,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="357"/>
-      <c r="P16" s="358"/>
+      <c r="O16" s="367"/>
+      <c r="P16" s="368"/>
     </row>
     <row r="17" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
@@ -10621,8 +10611,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="359"/>
-      <c r="P18" s="360"/>
+      <c r="O18" s="369"/>
+      <c r="P18" s="370"/>
     </row>
     <row r="19" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -11097,10 +11087,10 @@
     <row r="33" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="70"/>
       <c r="D33" s="72"/>
-      <c r="F33" s="333" t="s">
+      <c r="F33" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="333"/>
+      <c r="G33" s="352"/>
       <c r="H33" s="73">
         <f>SUM(H5:H26)</f>
         <v>36939.64</v>
@@ -11125,6 +11115,11 @@
     <sortCondition ref="B27:B30"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O18:P18"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="F2:H2"/>
@@ -11133,11 +11128,6 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O18:P18"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.15748031496062992" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11177,10 +11167,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -11192,15 +11182,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347" t="s">
+      <c r="B2" s="344" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -11210,32 +11200,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -11257,7 +11247,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -11516,8 +11506,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="355"/>
-      <c r="P11" s="356"/>
+      <c r="O11" s="365"/>
+      <c r="P11" s="366"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
@@ -11687,8 +11677,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="357"/>
-      <c r="P16" s="358"/>
+      <c r="O16" s="367"/>
+      <c r="P16" s="368"/>
     </row>
     <row r="17" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
@@ -11749,8 +11739,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="359"/>
-      <c r="P18" s="360"/>
+      <c r="O18" s="369"/>
+      <c r="P18" s="370"/>
     </row>
     <row r="19" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -12260,10 +12250,10 @@
     <row r="34" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="70"/>
       <c r="D34" s="72"/>
-      <c r="F34" s="333" t="s">
+      <c r="F34" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="333"/>
+      <c r="G34" s="352"/>
       <c r="H34" s="73">
         <f>SUM(H5:H27)</f>
         <v>42297.960000000006</v>
@@ -12288,11 +12278,6 @@
     <sortCondition ref="B6:B31"/>
   </sortState>
   <mergeCells count="13">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -12301,6 +12286,11 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.16" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12340,10 +12330,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -12355,15 +12345,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347" t="s">
+      <c r="B2" s="344" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -12373,32 +12363,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -12420,7 +12410,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -12473,10 +12463,10 @@
         <f>L5-I5</f>
         <v>-1</v>
       </c>
-      <c r="O5" s="372" t="s">
+      <c r="O5" s="382" t="s">
         <v>71</v>
       </c>
-      <c r="P5" s="373"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -12514,10 +12504,10 @@
         <f t="shared" ref="N6:N9" si="2">L6-I6</f>
         <v>-20</v>
       </c>
-      <c r="O6" s="364" t="s">
+      <c r="O6" s="374" t="s">
         <v>70</v>
       </c>
-      <c r="P6" s="365"/>
+      <c r="P6" s="375"/>
     </row>
     <row r="7" spans="2:16" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
@@ -12594,10 +12584,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O8" s="374" t="s">
+      <c r="O8" s="384" t="s">
         <v>80</v>
       </c>
-      <c r="P8" s="375"/>
+      <c r="P8" s="385"/>
     </row>
     <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -12670,10 +12660,10 @@
         <f t="shared" ref="N10" si="4">L10-I10</f>
         <v>-1</v>
       </c>
-      <c r="O10" s="366" t="s">
+      <c r="O10" s="376" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="367"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -12789,8 +12779,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O13" s="355"/>
-      <c r="P13" s="356"/>
+      <c r="O13" s="365"/>
+      <c r="P13" s="366"/>
     </row>
     <row r="14" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -12960,8 +12950,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O18" s="357"/>
-      <c r="P18" s="358"/>
+      <c r="O18" s="367"/>
+      <c r="P18" s="368"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -13030,8 +13020,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O20" s="362"/>
-      <c r="P20" s="363"/>
+      <c r="O20" s="372"/>
+      <c r="P20" s="373"/>
     </row>
     <row r="21" spans="2:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -13073,10 +13063,10 @@
         <f t="shared" si="5"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="368" t="s">
+      <c r="O21" s="378" t="s">
         <v>73</v>
       </c>
-      <c r="P21" s="369"/>
+      <c r="P21" s="379"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -13180,10 +13170,10 @@
         <f t="shared" si="5"/>
         <v>-21</v>
       </c>
-      <c r="O24" s="370" t="s">
+      <c r="O24" s="380" t="s">
         <v>72</v>
       </c>
-      <c r="P24" s="371"/>
+      <c r="P24" s="381"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
@@ -13466,10 +13456,10 @@
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
-      <c r="O32" s="368" t="s">
+      <c r="O32" s="378" t="s">
         <v>74</v>
       </c>
-      <c r="P32" s="369"/>
+      <c r="P32" s="379"/>
     </row>
     <row r="33" spans="2:16" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="165" t="s">
@@ -13565,10 +13555,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="333" t="s">
+      <c r="F36" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="333"/>
+      <c r="G36" s="352"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>55685.099999999991</v>
@@ -13593,6 +13583,11 @@
     <sortCondition ref="B5:B34"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -13608,11 +13603,6 @@
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13652,10 +13642,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -13667,15 +13657,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347" t="s">
+      <c r="B2" s="344" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -13685,32 +13675,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -13732,7 +13722,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -13781,8 +13771,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="372"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="382"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -13820,8 +13810,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="364"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -13908,8 +13898,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="376"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="386"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -13970,10 +13960,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="366" t="s">
+      <c r="O10" s="376" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="367"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -14093,8 +14083,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="355"/>
-      <c r="P13" s="356"/>
+      <c r="O13" s="365"/>
+      <c r="P13" s="366"/>
     </row>
     <row r="14" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="21" t="s">
@@ -14264,8 +14254,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="357"/>
-      <c r="P18" s="358"/>
+      <c r="O18" s="367"/>
+      <c r="P18" s="368"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
@@ -14334,8 +14324,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="362"/>
-      <c r="P20" s="363"/>
+      <c r="O20" s="372"/>
+      <c r="P20" s="373"/>
     </row>
     <row r="21" spans="2:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -14377,10 +14367,10 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="368" t="s">
+      <c r="O21" s="378" t="s">
         <v>79</v>
       </c>
-      <c r="P21" s="369"/>
+      <c r="P21" s="379"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -14488,8 +14478,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="370"/>
-      <c r="P24" s="371"/>
+      <c r="O24" s="380"/>
+      <c r="P24" s="381"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="21" t="s">
@@ -14760,10 +14750,10 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="O32" s="368" t="s">
+      <c r="O32" s="378" t="s">
         <v>78</v>
       </c>
-      <c r="P32" s="369"/>
+      <c r="P32" s="379"/>
     </row>
     <row r="33" spans="2:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="165" t="s">
@@ -14859,10 +14849,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="333" t="s">
+      <c r="F36" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="333"/>
+      <c r="G36" s="352"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>56083.79800000001</v>
@@ -14884,14 +14874,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -14904,6 +14886,14 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.15748031496062992" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14943,10 +14933,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -14958,15 +14948,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347" t="s">
+      <c r="B2" s="344" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -14976,32 +14966,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -15023,7 +15013,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -15072,8 +15062,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="372"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="382"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -15103,8 +15093,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="364"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -15179,8 +15169,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="376"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="386"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -15245,10 +15235,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="366" t="s">
+      <c r="O10" s="376" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="367"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -15364,8 +15354,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="355"/>
-      <c r="P13" s="356"/>
+      <c r="O13" s="365"/>
+      <c r="P13" s="366"/>
     </row>
     <row r="14" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -15535,8 +15525,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="357"/>
-      <c r="P18" s="358"/>
+      <c r="O18" s="367"/>
+      <c r="P18" s="368"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -15605,8 +15595,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="362"/>
-      <c r="P20" s="363"/>
+      <c r="O20" s="372"/>
+      <c r="P20" s="373"/>
     </row>
     <row r="21" spans="2:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -15644,10 +15634,10 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="368" t="s">
+      <c r="O21" s="378" t="s">
         <v>79</v>
       </c>
-      <c r="P21" s="369"/>
+      <c r="P21" s="379"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -15751,8 +15741,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="370"/>
-      <c r="P24" s="371"/>
+      <c r="O24" s="380"/>
+      <c r="P24" s="381"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
@@ -16015,10 +16005,10 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="O32" s="368" t="s">
+      <c r="O32" s="378" t="s">
         <v>78</v>
       </c>
-      <c r="P32" s="369"/>
+      <c r="P32" s="379"/>
     </row>
     <row r="33" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B33" s="165" t="s">
@@ -16114,10 +16104,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="333" t="s">
+      <c r="F36" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="333"/>
+      <c r="G36" s="352"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>23272.91</v>
@@ -16139,14 +16129,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -16159,6 +16141,14 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.43307086614173229" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16198,10 +16188,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -16213,15 +16203,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347">
+      <c r="B2" s="344">
         <v>44444</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -16231,32 +16221,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -16278,7 +16268,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -16327,8 +16317,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="372"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="382"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -16366,8 +16356,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="364"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -16442,8 +16432,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="376"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="386"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -16504,10 +16494,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="366" t="s">
+      <c r="O10" s="376" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="367"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -16623,8 +16613,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="355"/>
-      <c r="P13" s="356"/>
+      <c r="O13" s="365"/>
+      <c r="P13" s="366"/>
     </row>
     <row r="14" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -16802,8 +16792,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="357"/>
-      <c r="P18" s="358"/>
+      <c r="O18" s="367"/>
+      <c r="P18" s="368"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -16872,8 +16862,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="362"/>
-      <c r="P20" s="363"/>
+      <c r="O20" s="372"/>
+      <c r="P20" s="373"/>
     </row>
     <row r="21" spans="2:16" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -16911,10 +16901,10 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="378" t="s">
+      <c r="O21" s="388" t="s">
         <v>88</v>
       </c>
-      <c r="P21" s="379"/>
+      <c r="P21" s="389"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -17018,8 +17008,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O24" s="370"/>
-      <c r="P24" s="371"/>
+      <c r="O24" s="380"/>
+      <c r="P24" s="381"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
@@ -17379,10 +17369,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="333" t="s">
+      <c r="F36" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="333"/>
+      <c r="G36" s="352"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>32951.5</v>
@@ -17407,6 +17397,13 @@
     <sortCondition ref="B15:B18"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -17419,13 +17416,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.15748031496062992" top="0.43307086614173229" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17465,10 +17455,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="346" t="s">
+      <c r="B1" s="343" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="346"/>
+      <c r="C1" s="343"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -17480,15 +17470,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="347">
+      <c r="B2" s="344">
         <v>44472</v>
       </c>
-      <c r="C2" s="348"/>
-      <c r="F2" s="361" t="s">
+      <c r="C2" s="345"/>
+      <c r="F2" s="371" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="361"/>
-      <c r="H2" s="361"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -17498,32 +17488,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="349" t="s">
+      <c r="C3" s="346" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="350"/>
+      <c r="D3" s="347"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="351" t="s">
+      <c r="F3" s="348" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="352"/>
+      <c r="G3" s="349"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="353" t="s">
+      <c r="I3" s="350" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="338" t="s">
+      <c r="K3" s="357" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="339"/>
-      <c r="M3" s="334" t="s">
+      <c r="L3" s="358"/>
+      <c r="M3" s="353" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="335"/>
-      <c r="O3" s="336" t="s">
+      <c r="N3" s="354"/>
+      <c r="O3" s="355" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="337"/>
+      <c r="P3" s="356"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -17545,7 +17535,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="354"/>
+      <c r="I4" s="351"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -17594,8 +17584,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="372"/>
-      <c r="P5" s="373"/>
+      <c r="O5" s="382"/>
+      <c r="P5" s="383"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -17633,8 +17623,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="364"/>
-      <c r="P6" s="365"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="375"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -17709,8 +17699,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="376"/>
-      <c r="P8" s="377"/>
+      <c r="O8" s="386"/>
+      <c r="P8" s="387"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
@@ -17787,8 +17777,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="366"/>
-      <c r="P10" s="367"/>
+      <c r="O10" s="376"/>
+      <c r="P10" s="377"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="164" t="s">
@@ -17939,8 +17929,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="355"/>
-      <c r="P14" s="356"/>
+      <c r="O14" s="365"/>
+      <c r="P14" s="366"/>
     </row>
     <row r="15" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
@@ -18110,8 +18100,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="357"/>
-      <c r="P19" s="358"/>
+      <c r="O19" s="367"/>
+      <c r="P19" s="368"/>
     </row>
     <row r="20" spans="2:18" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
@@ -18172,8 +18162,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="362"/>
-      <c r="P21" s="363"/>
+      <c r="O21" s="372"/>
+      <c r="P21" s="373"/>
     </row>
     <row r="22" spans="2:18" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -18215,14 +18205,14 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O22" s="368" t="s">
+      <c r="O22" s="378" t="s">
         <v>88</v>
       </c>
-      <c r="P22" s="369"/>
-      <c r="Q22" s="380" t="s">
+      <c r="P22" s="379"/>
+      <c r="Q22" s="390" t="s">
         <v>95</v>
       </c>
-      <c r="R22" s="381"/>
+      <c r="R22" s="391"/>
     </row>
     <row r="23" spans="2:18" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
@@ -18262,8 +18252,8 @@
       </c>
       <c r="O23" s="191"/>
       <c r="P23" s="192"/>
-      <c r="Q23" s="380"/>
-      <c r="R23" s="381"/>
+      <c r="Q23" s="390"/>
+      <c r="R23" s="391"/>
     </row>
     <row r="24" spans="2:18" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="21" t="s">
@@ -18324,8 +18314,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25" s="370"/>
-      <c r="P25" s="371"/>
+      <c r="O25" s="380"/>
+      <c r="P25" s="381"/>
     </row>
     <row r="26" spans="2:18" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
@@ -18693,10 +18683,10 @@
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="333" t="s">
+      <c r="F37" s="352" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="333"/>
+      <c r="G37" s="352"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>61770.95</v>
@@ -18721,13 +18711,6 @@
     <sortCondition ref="B9:B11"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q22:R23"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
@@ -18741,6 +18724,13 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.47244094488188981" right="0.15748031496062992" top="0.35433070866141736" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>